<commit_message>
push testcases from 2 to 15
</commit_message>
<xml_diff>
--- a/excel_data/data.xlsx
+++ b/excel_data/data.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zafar\eclipse-workspace\Amazon_Pom_project\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B139CC-530A-4ECC-B7C7-B7BC5B6ECD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE85154-7C0F-4846-B0C5-DEE37D017418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="search_product" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Incorrect_login" sheetId="3" r:id="rId3"/>
+    <sheet name="profile" sheetId="4" r:id="rId4"/>
+    <sheet name="Price_range_handler" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,22 +29,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>toy</t>
   </si>
+  <si>
+    <t>zafar</t>
+  </si>
+  <si>
+    <t>zafar shareef</t>
+  </si>
+  <si>
+    <t>Sport &amp; Outdoor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -63,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,7 +367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -361,4 +381,113 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA4C049-6A87-4C57-92D7-D816C956ED67}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.21875" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>9131899877</v>
+      </c>
+      <c r="B1">
+        <v>9131899877</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754C2648-E93D-4542-A6E5-698265AB7EC8}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="3" width="38.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>9131899877</v>
+      </c>
+      <c r="B1">
+        <v>9131899856</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB4D733-FF98-42E4-BA62-461D45EF8357}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC917BB-FD87-4BBF-B1E5-F837379A15D6}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>